<commit_message>
Add and use SubBucket to all RiskClasses that might ever use it.
</commit_message>
<xml_diff>
--- a/Configs/FRTBConfig_BCBS.xlsx
+++ b/Configs/FRTBConfig_BCBS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alan/Workspace/FRTB/Configs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B527F111-DC44-BF40-B28C-950E82D18231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181BE14E-CCF2-0343-8D93-B7AF055F36DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="1400" windowWidth="29640" windowHeight="22340" xr2:uid="{702274BA-38C3-0147-8564-8B67C0FD49FC}"/>
+    <workbookView xWindow="10560" yWindow="4720" windowWidth="40140" windowHeight="26920" activeTab="3" xr2:uid="{702274BA-38C3-0147-8564-8B67C0FD49FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Copyright" sheetId="22" r:id="rId1"/>
@@ -36,7 +36,7 @@
   </sheets>
   <definedNames>
     <definedName name="fna_MAR_21_51_15" localSheetId="3">MS_CR!$E$9</definedName>
-    <definedName name="fna_MAR_21_51_16" localSheetId="3">MS_CR!$E$17</definedName>
+    <definedName name="fna_MAR_21_51_16" localSheetId="3">MS_CR!$E$18</definedName>
     <definedName name="fna_MAR_21_62_19" localSheetId="5">MS_CS!$D$26</definedName>
     <definedName name="fna_MAR_21_72_20" localSheetId="6">MS_EQ!$F$12</definedName>
   </definedNames>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="248">
   <si>
     <t>Bucket</t>
   </si>
@@ -740,9 +740,6 @@
     <t>DeltaNameBucketRho</t>
   </si>
   <si>
-    <t>DeltaCovBondAARiskWeight</t>
-  </si>
-  <si>
     <t>CoveredBondBucket</t>
   </si>
   <si>
@@ -849,6 +846,18 @@
   </si>
   <si>
     <t>along with this program. If not, see &lt;https://www.gnu.org/licenses/&gt;.</t>
+  </si>
+  <si>
+    <t>8a</t>
+  </si>
+  <si>
+    <t>8b</t>
+  </si>
+  <si>
+    <t>Covered bonds - High Quality</t>
+  </si>
+  <si>
+    <t>Covered bonds - Not High Quality</t>
   </si>
 </sst>
 </file>
@@ -1281,15 +1290,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D95B6A-2092-4D43-ABCB-456863E81D66}">
   <dimension ref="A1:A17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -1297,7 +1304,7 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:1">
@@ -1308,22 +1315,22 @@
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="10" spans="1:1">
@@ -1331,22 +1338,22 @@
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:1">
@@ -1354,12 +1361,12 @@
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -1487,7 +1494,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="B15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C15">
         <v>0.15</v>
@@ -1495,7 +1502,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="B16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1503,7 +1510,7 @@
     </row>
     <row r="17" spans="2:3">
       <c r="B17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1587,7 +1594,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="B8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C8">
         <v>0.15</v>
@@ -1595,7 +1602,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="B9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1603,7 +1610,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="B10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1742,10 +1749,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B1" t="s">
         <v>213</v>
-      </c>
-      <c r="B1" t="s">
-        <v>214</v>
       </c>
       <c r="C1">
         <v>0.01</v>
@@ -1753,7 +1760,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="B2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C2">
         <v>1E-3</v>
@@ -1971,7 +1978,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
@@ -1987,7 +1994,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B18" s="1">
         <v>0.8</v>
@@ -2003,7 +2010,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B19" s="1">
         <v>0.5</v>
@@ -2019,7 +2026,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B20" s="1">
         <v>0.7</v>
@@ -2035,7 +2042,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B21">
         <v>0.01</v>
@@ -2043,7 +2050,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -2097,7 +2104,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B3">
         <v>1.5800000000000002E-2</v>
@@ -2105,7 +2112,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B4">
         <v>1.5800000000000002E-2</v>
@@ -2441,7 +2448,7 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B11">
         <v>8</v>
@@ -5049,9 +5056,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD33"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -5063,7 +5068,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B1" t="s">
         <v>49</v>
@@ -6303,9 +6308,9 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02F955FF-3809-B846-9AD2-659C7F98C4D6}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:S51"/>
+  <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -6420,199 +6425,216 @@
       <c r="B9" s="3">
         <v>8</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>144</v>
+      </c>
       <c r="D9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>16</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="B10" s="3">
-        <v>9</v>
-      </c>
-      <c r="C10" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>145</v>
+      </c>
       <c r="D10" s="3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>7</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="B11" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="B12" s="3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="B13" s="3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="B14" s="3">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="B15" s="3">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="B16" s="3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E16" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="B17" s="3">
+        <v>15</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:19">
-      <c r="B17" s="3">
+    <row r="18" spans="1:20">
+      <c r="B18" s="3">
         <v>16</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="E17" s="3" t="s">
+      <c r="C18" s="3"/>
+      <c r="E18" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:19">
-      <c r="B18" s="3">
+    <row r="19" spans="1:20">
+      <c r="B19" s="3">
         <v>17</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19">
-      <c r="B19" s="3">
-        <v>18</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="20" spans="1:19">
-      <c r="A20" t="s">
+    <row r="20" spans="1:20">
+      <c r="B20" s="3">
+        <v>18</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="I20" t="s">
+        <v>244</v>
+      </c>
+      <c r="J20" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" t="s">
         <v>151</v>
       </c>
-      <c r="B20">
+      <c r="B21">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C20">
+      <c r="C21">
         <v>0.01</v>
       </c>
-      <c r="D20">
-        <v>0.05</v>
-      </c>
-      <c r="E20">
+      <c r="D21">
+        <v>0.05</v>
+      </c>
+      <c r="E21">
         <v>0.03</v>
       </c>
-      <c r="F20">
+      <c r="F21">
         <v>0.03</v>
       </c>
-      <c r="G20">
+      <c r="G21">
         <v>0.02</v>
       </c>
-      <c r="H20">
+      <c r="H21">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="I20">
+      <c r="I21" s="3">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J21">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="J20">
+      <c r="K21">
         <v>0.02</v>
       </c>
-      <c r="K20">
+      <c r="L21">
         <v>0.04</v>
       </c>
-      <c r="L20">
+      <c r="M21">
         <v>0.12</v>
       </c>
-      <c r="M20">
+      <c r="N21">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="N20">
+      <c r="O21">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="O20">
+      <c r="P21">
         <v>5.5E-2</v>
       </c>
-      <c r="P20">
-        <v>0.05</v>
-      </c>
-      <c r="Q20">
+      <c r="Q21">
+        <v>0.05</v>
+      </c>
+      <c r="R21">
         <v>0.12</v>
       </c>
-      <c r="R20">
+      <c r="S21">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="S20">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19">
-      <c r="A21" t="s">
-        <v>208</v>
-      </c>
-      <c r="B21" s="3">
-        <v>1.4999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19">
+      <c r="T21">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
       <c r="A22" t="s">
         <v>160</v>
       </c>
@@ -6620,7 +6642,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:20">
       <c r="A23" t="s">
         <v>156</v>
       </c>
@@ -6628,7 +6650,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:20">
       <c r="A24" t="s">
         <v>155</v>
       </c>
@@ -6636,7 +6658,7 @@
         <v>0.999</v>
       </c>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:20">
       <c r="A25" t="s">
         <v>161</v>
       </c>
@@ -6644,7 +6666,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:20">
       <c r="A26" t="s">
         <v>162</v>
       </c>
@@ -6652,7 +6674,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:20">
       <c r="A27" t="s">
         <v>163</v>
       </c>
@@ -6660,38 +6682,38 @@
         <v>0.999</v>
       </c>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:20">
       <c r="A28" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B28">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:20">
       <c r="A29" t="s">
+        <v>218</v>
+      </c>
+      <c r="B29" t="s">
         <v>219</v>
-      </c>
-      <c r="B29" t="s">
-        <v>220</v>
       </c>
       <c r="C29" t="s">
         <v>102</v>
       </c>
       <c r="D29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E29" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F29" t="s">
         <v>101</v>
       </c>
       <c r="G29" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" ht="18">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" ht="18">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -6702,9 +6724,9 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:20">
       <c r="A31" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B31">
         <v>17</v>
@@ -6713,7 +6735,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:20">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -9626,13 +9648,13 @@
         <v>43</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>17</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:9">

</xml_diff>

<commit_message>
Add config for SIngaporre MAS.  Make MD_CS configs specify buckets (as with SG-MAS doc)
</commit_message>
<xml_diff>
--- a/Configs/FRTBConfig_BCBS.xlsx
+++ b/Configs/FRTBConfig_BCBS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alan/Workspace/FRTB/Configs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181BE14E-CCF2-0343-8D93-B7AF055F36DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08997159-1E7C-5247-85BB-940817035216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10560" yWindow="4720" windowWidth="40140" windowHeight="26920" activeTab="3" xr2:uid="{702274BA-38C3-0147-8564-8B67C0FD49FC}"/>
+    <workbookView xWindow="76820" yWindow="10600" windowWidth="40140" windowHeight="26920" activeTab="11" xr2:uid="{702274BA-38C3-0147-8564-8B67C0FD49FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Copyright" sheetId="22" r:id="rId1"/>
@@ -37,7 +37,7 @@
   <definedNames>
     <definedName name="fna_MAR_21_51_15" localSheetId="3">MS_CR!$E$9</definedName>
     <definedName name="fna_MAR_21_51_16" localSheetId="3">MS_CR!$E$18</definedName>
-    <definedName name="fna_MAR_21_62_19" localSheetId="5">MS_CS!$D$26</definedName>
+    <definedName name="fna_MAR_21_62_19" localSheetId="5">MS_CS!$E$26</definedName>
     <definedName name="fna_MAR_21_72_20" localSheetId="6">MS_EQ!$F$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="251">
   <si>
     <t>Bucket</t>
   </si>
@@ -440,15 +440,6 @@
     <t>CCC</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>OtherBucketSector</t>
-  </si>
-  <si>
-    <t>OtherBucketRegion</t>
-  </si>
-  <si>
     <t>Asia</t>
   </si>
   <si>
@@ -458,36 +449,6 @@
     <t>North America</t>
   </si>
   <si>
-    <t>Asset Backed CP</t>
-  </si>
-  <si>
-    <t>Auto Loas / Leases</t>
-  </si>
-  <si>
-    <t>RMBS</t>
-  </si>
-  <si>
-    <t>Credit Cards</t>
-  </si>
-  <si>
-    <t>CLO</t>
-  </si>
-  <si>
-    <t>CDO-Squared</t>
-  </si>
-  <si>
-    <t>SME</t>
-  </si>
-  <si>
-    <t>Student Loans</t>
-  </si>
-  <si>
-    <t>Oher Retal</t>
-  </si>
-  <si>
-    <t>Wholesale</t>
-  </si>
-  <si>
     <t>BA-Rho</t>
   </si>
   <si>
@@ -560,12 +521,6 @@
     <t>Sovereigns including central banks,multilateral development banks</t>
   </si>
   <si>
-    <t>IG Indices</t>
-  </si>
-  <si>
-    <t>HY Indices</t>
-  </si>
-  <si>
     <t>Local government,  government-backed non-financials,  education and public administration</t>
   </si>
   <si>
@@ -704,9 +659,6 @@
     <t>RUB</t>
   </si>
   <si>
-    <t>HKG</t>
-  </si>
-  <si>
     <t>SGD</t>
   </si>
   <si>
@@ -858,6 +810,63 @@
   </si>
   <si>
     <t>Covered bonds - Not High Quality</t>
+  </si>
+  <si>
+    <t>HKD</t>
+  </si>
+  <si>
+    <t># for Vega Risk weighting both bucket 12 and 13 are deemed Large Cap</t>
+  </si>
+  <si>
+    <t>Qualified indices</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>All Regions</t>
+  </si>
+  <si>
+    <t>Companies (excluding small businesses)</t>
+  </si>
+  <si>
+    <t>Asset-backed commercial paper</t>
+  </si>
+  <si>
+    <t>Auto loans and auto leases</t>
+  </si>
+  <si>
+    <t>Residential mortgage-backed securities (RMBS)</t>
+  </si>
+  <si>
+    <t>Credit cards</t>
+  </si>
+  <si>
+    <t>Commercial MBS</t>
+  </si>
+  <si>
+    <t>Collateralised loan obligations</t>
+  </si>
+  <si>
+    <t>Collateralised debt obligations (CDO)-squared</t>
+  </si>
+  <si>
+    <t>Companies which are small businesses</t>
+  </si>
+  <si>
+    <t>Student loans</t>
+  </si>
+  <si>
+    <t>Other retail</t>
+  </si>
+  <si>
+    <t>Other wholesale</t>
+  </si>
+  <si>
+    <t>All other</t>
+  </si>
+  <si>
+    <t>Others</t>
   </si>
 </sst>
 </file>
@@ -992,9 +1001,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1032,7 +1041,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1138,7 +1147,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1280,7 +1289,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1290,13 +1299,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D95B6A-2092-4D43-ABCB-456863E81D66}">
   <dimension ref="A1:A17"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="10" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -1304,7 +1315,7 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="10" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:1">
@@ -1315,22 +1326,22 @@
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="10" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="10" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="10" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="10" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10" spans="1:1">
@@ -1338,22 +1349,22 @@
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="10" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="10" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="10" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="10" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15" spans="1:1">
@@ -1361,12 +1372,12 @@
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="10" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="10" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -1430,7 +1441,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="B7" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1494,7 +1505,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="B15" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="C15">
         <v>0.15</v>
@@ -1502,7 +1513,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="B16" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1510,7 +1521,7 @@
     </row>
     <row r="17" spans="2:3">
       <c r="B17" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1594,7 +1605,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="B8" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="C8">
         <v>0.15</v>
@@ -1602,7 +1613,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="B9" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1610,7 +1621,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="B10" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1624,9 +1635,9 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5213FE0F-D032-134C-8CBD-C9C991BBB3F3}">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -1634,103 +1645,524 @@
     <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="B2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="B3" t="s">
+      <c r="C1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="D3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>109</v>
+      </c>
+      <c r="D17" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D20" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>109</v>
+      </c>
+      <c r="D21" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
         <v>110</v>
       </c>
-      <c r="B4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="B5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="B6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="B7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>109</v>
-      </c>
-      <c r="B8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="B9" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="B10" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="B11" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="B13" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="B14" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="B15" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="B16" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2">
-      <c r="B18" t="s">
-        <v>123</v>
+      <c r="D25" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29" t="s">
+        <v>110</v>
+      </c>
+      <c r="D29" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30" t="s">
+        <v>110</v>
+      </c>
+      <c r="D30" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32" t="s">
+        <v>110</v>
+      </c>
+      <c r="D32" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34" t="s">
+        <v>110</v>
+      </c>
+      <c r="D34" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4">
+      <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4">
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36" t="s">
+        <v>249</v>
+      </c>
+      <c r="D36" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4">
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37" t="s">
+        <v>249</v>
+      </c>
+      <c r="D37" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4">
+      <c r="B38">
+        <v>37</v>
+      </c>
+      <c r="C38" t="s">
+        <v>249</v>
+      </c>
+      <c r="D38" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4">
+      <c r="B39">
+        <v>38</v>
+      </c>
+      <c r="C39" t="s">
+        <v>249</v>
+      </c>
+      <c r="D39" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4">
+      <c r="B40">
+        <v>39</v>
+      </c>
+      <c r="C40" t="s">
+        <v>249</v>
+      </c>
+      <c r="D40" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4">
+      <c r="B41">
+        <v>40</v>
+      </c>
+      <c r="C41" t="s">
+        <v>249</v>
+      </c>
+      <c r="D41" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4">
+      <c r="B42">
+        <v>41</v>
+      </c>
+      <c r="C42" t="s">
+        <v>249</v>
+      </c>
+      <c r="D42" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4">
+      <c r="B43">
+        <v>42</v>
+      </c>
+      <c r="C43" t="s">
+        <v>249</v>
+      </c>
+      <c r="D43" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4">
+      <c r="B44">
+        <v>43</v>
+      </c>
+      <c r="C44" t="s">
+        <v>249</v>
+      </c>
+      <c r="D44" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4">
+      <c r="B45">
+        <v>44</v>
+      </c>
+      <c r="C45" t="s">
+        <v>249</v>
+      </c>
+      <c r="D45" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4">
+      <c r="B46">
+        <v>45</v>
+      </c>
+      <c r="C46" t="s">
+        <v>249</v>
+      </c>
+      <c r="D46" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4">
+      <c r="B47">
+        <v>46</v>
+      </c>
+      <c r="C47" t="s">
+        <v>236</v>
+      </c>
+      <c r="D47" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -1749,10 +2181,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="B1" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="C1">
         <v>0.01</v>
@@ -1760,7 +2192,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="B2" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="C2">
         <v>1E-3</v>
@@ -1785,7 +2217,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="B1">
         <v>0.5</v>
@@ -1793,7 +2225,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1801,7 +2233,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="B3">
         <v>1.4</v>
@@ -1809,7 +2241,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="B4">
         <v>0.25</v>
@@ -1817,7 +2249,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B5">
         <v>0.65</v>
@@ -1825,13 +2257,13 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -1840,7 +2272,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1850,7 +2282,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1917,68 +2349,68 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>0.01</v>
       </c>
-      <c r="E15" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="F15" s="2">
+      <c r="E15" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="F15" s="1">
         <v>0.03</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="1">
         <v>0.03</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="1">
         <v>0.02</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="1">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="1">
         <v>0.05</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="B16" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C16" s="2">
+        <v>118</v>
+      </c>
+      <c r="C16" s="1">
         <v>0.02</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>0.04</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="1">
         <v>0.12</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="1">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="1">
         <v>5.5E-2</v>
       </c>
-      <c r="I16" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="J16" s="2">
+      <c r="I16" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="J16" s="1">
         <v>0.12</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
@@ -1994,7 +2426,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
       <c r="B18" s="1">
         <v>0.8</v>
@@ -2010,7 +2442,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="B19" s="1">
         <v>0.5</v>
@@ -2026,7 +2458,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="B20" s="1">
         <v>0.7</v>
@@ -2042,7 +2474,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="B21">
         <v>0.01</v>
@@ -2050,7 +2482,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -2076,7 +2508,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="B1">
         <v>1.11E-2</v>
@@ -2096,7 +2528,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="B2">
         <v>1.11E-2</v>
@@ -2104,7 +2536,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="B3">
         <v>1.5800000000000002E-2</v>
@@ -2112,7 +2544,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="B4">
         <v>1.5800000000000002E-2</v>
@@ -2129,24 +2561,24 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="E5" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="F5" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="G5" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="H5" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="B6" s="3">
         <v>1</v>
@@ -2235,7 +2667,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="B11" s="3">
         <v>0.4</v>
@@ -2243,7 +2675,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="B12" s="3">
         <v>0.4</v>
@@ -2259,7 +2691,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B14" s="3">
         <v>1</v>
@@ -2267,7 +2699,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="B15" s="3">
         <v>0.4</v>
@@ -2312,7 +2744,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="B1">
         <v>0.11</v>
@@ -2320,7 +2752,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2362,7 +2794,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
@@ -2373,10 +2805,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="D2" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -2384,10 +2816,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -2443,12 +2875,12 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
       <c r="B11">
         <v>8</v>
@@ -2456,7 +2888,7 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
@@ -2491,7 +2923,7 @@
     </row>
     <row r="13" spans="1:11">
       <c r="B13" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="C13">
         <v>0.02</v>
@@ -2523,7 +2955,7 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="B14">
         <v>0.9</v>
@@ -2531,7 +2963,7 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="B15">
         <v>0.5</v>
@@ -2539,7 +2971,7 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="B16">
         <v>0.9</v>
@@ -2547,7 +2979,7 @@
     </row>
     <row r="17" spans="1:19">
       <c r="A17" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="B17">
         <v>0.8</v>
@@ -2555,7 +2987,7 @@
     </row>
     <row r="18" spans="1:19">
       <c r="A18" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="B18">
         <v>0.9</v>
@@ -2563,7 +2995,7 @@
     </row>
     <row r="19" spans="1:19">
       <c r="A19" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="B19">
         <v>0.8</v>
@@ -2571,7 +3003,7 @@
     </row>
     <row r="20" spans="1:19">
       <c r="A20" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="B20">
         <v>0.9</v>
@@ -2579,7 +3011,7 @@
     </row>
     <row r="21" spans="1:19">
       <c r="A21" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="B21">
         <v>0.8</v>
@@ -2883,7 +3315,7 @@
   <dimension ref="A1:R37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="O19" sqref="O19:R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2901,7 +3333,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
@@ -2929,7 +3361,7 @@
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2992,7 +3424,7 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
@@ -3003,10 +3435,10 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="E10" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -3014,7 +3446,7 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
@@ -3025,7 +3457,7 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -3036,7 +3468,7 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
@@ -3047,7 +3479,7 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="E14" t="s">
         <v>12</v>
@@ -3058,7 +3490,7 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="E15" t="s">
         <v>13</v>
@@ -3068,7 +3500,7 @@
       <c r="B16">
         <v>15</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3077,7 +3509,10 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>148</v>
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -3085,12 +3520,15 @@
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>149</v>
+        <v>118</v>
+      </c>
+      <c r="E18" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="19" spans="1:18">
       <c r="A19" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="B19">
         <v>5.0000000000000001E-3</v>
@@ -3146,7 +3584,7 @@
     </row>
     <row r="20" spans="1:18">
       <c r="A20" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -4064,11 +4502,9 @@
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB646BC-02D0-0A44-A321-CB438F3714FE}">
   <sheetPr codeName="Sheet18"/>
-  <dimension ref="A1:O48"/>
+  <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -4085,7 +4521,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>34</v>
@@ -4252,7 +4688,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -4262,6 +4698,12 @@
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>46</v>
       </c>
     </row>
@@ -4270,7 +4712,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="3"/>
-      <c r="D14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>47</v>
       </c>
     </row>
@@ -4365,7 +4807,7 @@
     </row>
     <row r="31" spans="1:14">
       <c r="A31" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="B31">
         <v>0.55000000000000004</v>
@@ -4409,7 +4851,7 @@
     </row>
     <row r="32" spans="1:14">
       <c r="A32" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="B32">
         <v>0.78</v>
@@ -4453,7 +4895,7 @@
     </row>
     <row r="33" spans="1:15">
       <c r="A33" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="B33">
         <v>0.15</v>
@@ -4495,26 +4937,57 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="18">
-      <c r="A34" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B34" s="4">
-        <v>11</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>33</v>
-      </c>
+    <row r="34" spans="1:15">
+      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0.15</v>
+      </c>
+      <c r="D34">
+        <v>0.15</v>
+      </c>
+      <c r="E34">
+        <v>0.15</v>
+      </c>
+      <c r="F34">
+        <v>0.15</v>
+      </c>
+      <c r="G34">
+        <v>0.15</v>
+      </c>
+      <c r="H34">
+        <v>0.15</v>
+      </c>
+      <c r="I34">
+        <v>0.15</v>
+      </c>
+      <c r="J34">
+        <v>0.15</v>
+      </c>
+      <c r="K34">
+        <v>0.15</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <v>0.45</v>
+      </c>
+      <c r="N34">
+        <v>0.45</v>
+      </c>
+      <c r="O34" s="3"/>
     </row>
     <row r="35" spans="1:15">
-      <c r="A35" t="s">
-        <v>3</v>
-      </c>
       <c r="B35">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="C35">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="D35">
         <v>0.15</v>
@@ -4549,17 +5022,16 @@
       <c r="N35">
         <v>0.45</v>
       </c>
-      <c r="O35" s="3"/>
     </row>
     <row r="36" spans="1:15">
       <c r="B36">
         <v>0.15</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="D36">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="E36">
         <v>0.15</v>
@@ -4600,10 +5072,10 @@
         <v>0.15</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="E37">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="F37">
         <v>0.15</v>
@@ -4644,10 +5116,10 @@
         <v>0.15</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="F38">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="G38">
         <v>0.15</v>
@@ -4688,10 +5160,10 @@
         <v>0.15</v>
       </c>
       <c r="F39">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="G39">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="H39">
         <v>0.15</v>
@@ -4732,10 +5204,10 @@
         <v>0.15</v>
       </c>
       <c r="G40">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="H40">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="I40">
         <v>0.15</v>
@@ -4776,10 +5248,10 @@
         <v>0.15</v>
       </c>
       <c r="H41">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="I41">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="J41">
         <v>0.15</v>
@@ -4820,10 +5292,10 @@
         <v>0.15</v>
       </c>
       <c r="I42">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J42">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="K42">
         <v>0.15</v>
@@ -4864,10 +5336,10 @@
         <v>0.15</v>
       </c>
       <c r="J43">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="K43">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="L43">
         <v>0</v>
@@ -4881,31 +5353,31 @@
     </row>
     <row r="44" spans="1:15">
       <c r="B44">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="C44">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="D44">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="E44">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="F44">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="G44">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="H44">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="I44">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="J44">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="K44">
         <v>0</v>
@@ -4914,42 +5386,42 @@
         <v>0</v>
       </c>
       <c r="M44">
-        <v>0.45</v>
+        <v>0</v>
       </c>
       <c r="N44">
-        <v>0.45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:15">
       <c r="B45">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="E45">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="F45">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="G45">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="H45">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="I45">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="J45">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="K45">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="L45">
         <v>0</v>
@@ -4958,7 +5430,7 @@
         <v>0</v>
       </c>
       <c r="N45">
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="46" spans="1:15">
@@ -4996,55 +5468,14 @@
         <v>0</v>
       </c>
       <c r="M46">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="N46">
-        <v>0.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:15">
-      <c r="B47">
-        <v>0.45</v>
-      </c>
-      <c r="C47">
-        <v>0.45</v>
-      </c>
-      <c r="D47">
-        <v>0.45</v>
-      </c>
-      <c r="E47">
-        <v>0.45</v>
-      </c>
-      <c r="F47">
-        <v>0.45</v>
-      </c>
-      <c r="G47">
-        <v>0.45</v>
-      </c>
-      <c r="H47">
-        <v>0.45</v>
-      </c>
-      <c r="I47">
-        <v>0.45</v>
-      </c>
-      <c r="J47">
-        <v>0.45</v>
-      </c>
-      <c r="K47">
-        <v>0.45</v>
-      </c>
-      <c r="L47">
-        <v>0</v>
-      </c>
-      <c r="M47">
-        <v>0.75</v>
-      </c>
-      <c r="N47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15">
-      <c r="B48" s="3"/>
+      <c r="B47" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5068,7 +5499,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
-        <v>231</v>
+        <v>215</v>
       </c>
       <c r="B1" t="s">
         <v>49</v>
@@ -5076,7 +5507,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="B2" s="3">
         <v>0.55000000000000004</v>
@@ -5084,7 +5515,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="B3" s="3">
         <v>0.01</v>
@@ -5092,21 +5523,21 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="B4" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="C4" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="D4" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="C5">
         <v>60</v>
@@ -5114,7 +5545,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="C6">
         <v>120</v>
@@ -5122,7 +5553,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="C7">
         <v>120</v>
@@ -5130,7 +5561,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="B8" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="C8">
         <v>120</v>
@@ -5138,7 +5569,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="B9" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="C9">
         <v>20</v>
@@ -5149,7 +5580,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="B10" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="C10">
         <v>60</v>
@@ -5160,7 +5591,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="B11" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="C11">
         <v>120</v>
@@ -5168,7 +5599,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="B12" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="C12">
         <v>40</v>
@@ -5200,7 +5631,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>69</v>
@@ -5343,7 +5774,7 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="B13">
         <v>0.3</v>
@@ -5381,7 +5812,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B14" s="3">
         <v>1</v>
@@ -5798,7 +6229,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="B1">
         <v>1.7000000000000001E-2</v>
@@ -5833,7 +6264,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="B2">
         <v>1.6E-2</v>
@@ -5841,7 +6272,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="B3">
         <v>1.6E-2</v>
@@ -5858,24 +6289,24 @@
         <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="E4" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="F4" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="G4" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="H4" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="B5" s="3">
         <v>0.03</v>
@@ -5883,7 +6314,7 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="B6" s="3">
         <v>0.01</v>
@@ -5891,7 +6322,7 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
@@ -6215,7 +6646,7 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="B17" s="3">
         <v>0.999</v>
@@ -6223,7 +6654,7 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="B18" s="3">
         <v>0.4</v>
@@ -6231,7 +6662,7 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="B19" s="3">
         <v>0</v>
@@ -6310,7 +6741,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -6328,7 +6759,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>4</v>
@@ -6426,13 +6857,13 @@
         <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -6440,13 +6871,13 @@
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -6551,7 +6982,7 @@
         <v>6</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
     </row>
     <row r="20" spans="1:20">
@@ -6563,18 +6994,18 @@
         <v>14</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="I20" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="J20" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="1:20">
       <c r="A21" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="B21">
         <v>5.0000000000000001E-3</v>
@@ -6636,7 +7067,7 @@
     </row>
     <row r="22" spans="1:20">
       <c r="A22" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="B22">
         <v>0.35</v>
@@ -6644,7 +7075,7 @@
     </row>
     <row r="23" spans="1:20">
       <c r="A23" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="B23">
         <v>0.65</v>
@@ -6652,7 +7083,7 @@
     </row>
     <row r="24" spans="1:20">
       <c r="A24" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="B24">
         <v>0.999</v>
@@ -6660,7 +7091,7 @@
     </row>
     <row r="25" spans="1:20">
       <c r="A25" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="B25">
         <v>0.8</v>
@@ -6668,7 +7099,7 @@
     </row>
     <row r="26" spans="1:20">
       <c r="A26" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="B26">
         <v>0.65</v>
@@ -6676,7 +7107,7 @@
     </row>
     <row r="27" spans="1:20">
       <c r="A27" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="B27">
         <v>0.999</v>
@@ -6684,7 +7115,7 @@
     </row>
     <row r="28" spans="1:20">
       <c r="A28" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="B28">
         <v>8</v>
@@ -6692,25 +7123,25 @@
     </row>
     <row r="29" spans="1:20">
       <c r="A29" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="B29" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="C29" t="s">
         <v>102</v>
       </c>
       <c r="D29" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="E29" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="F29" t="s">
         <v>101</v>
       </c>
       <c r="G29" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:20" ht="18">
@@ -6726,7 +7157,7 @@
     </row>
     <row r="31" spans="1:20">
       <c r="A31" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
       <c r="B31">
         <v>17</v>
@@ -7815,7 +8246,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>4</v>
@@ -8015,7 +8446,7 @@
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="B18">
         <v>0.04</v>
@@ -8068,7 +8499,7 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="B19">
         <v>0.35</v>
@@ -8076,7 +8507,7 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="B20">
         <v>0.65</v>
@@ -8084,7 +8515,7 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="B21">
         <v>0.99</v>
@@ -8962,7 +9393,9 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:Z34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -8980,7 +9413,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>4</v>
@@ -9282,13 +9715,13 @@
         <v>25</v>
       </c>
       <c r="C26" s="3"/>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:26">
       <c r="A27" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="B27">
         <v>8.9999999999999993E-3</v>
@@ -9368,7 +9801,7 @@
     </row>
     <row r="28" spans="1:26">
       <c r="A28" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="B28">
         <v>0.4</v>
@@ -9376,7 +9809,7 @@
     </row>
     <row r="29" spans="1:26">
       <c r="A29" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="B29">
         <v>0.8</v>
@@ -9384,7 +9817,7 @@
     </row>
     <row r="30" spans="1:26">
       <c r="A30" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="B30">
         <v>0.999</v>
@@ -9469,7 +9902,7 @@
     <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -9477,10 +9910,10 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>35</v>
@@ -9489,7 +9922,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="B2" s="3">
         <v>1</v>
       </c>
@@ -9504,7 +9937,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="B3" s="3">
         <v>2</v>
       </c>
@@ -9519,7 +9952,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="B4" s="3">
         <v>3</v>
       </c>
@@ -9534,7 +9967,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="B5" s="3">
         <v>4</v>
       </c>
@@ -9549,7 +9982,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="B6" s="3">
         <v>5</v>
       </c>
@@ -9564,7 +9997,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="B7" s="3">
         <v>6</v>
       </c>
@@ -9579,7 +10012,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="B8" s="3">
         <v>7</v>
       </c>
@@ -9594,7 +10027,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="B9" s="3">
         <v>8</v>
       </c>
@@ -9609,7 +10042,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="B10" s="3">
         <v>9</v>
       </c>
@@ -9624,7 +10057,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="B11" s="3">
         <v>10</v>
       </c>
@@ -9639,7 +10072,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:10">
       <c r="B12" s="3">
         <v>11</v>
       </c>
@@ -9648,16 +10081,16 @@
         <v>43</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="B13" s="3">
         <v>12</v>
       </c>
@@ -9669,10 +10102,10 @@
         <v>42</v>
       </c>
       <c r="F13" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="B14" s="3">
         <v>13</v>
       </c>
@@ -9680,11 +10113,14 @@
       <c r="D14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -9692,7 +10128,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -9775,7 +10211,7 @@
     </row>
     <row r="31" spans="1:15">
       <c r="A31" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>66</v>
@@ -9866,7 +10302,7 @@
     </row>
     <row r="33" spans="1:15">
       <c r="A33" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="B33">
         <v>0.15</v>
@@ -9910,7 +10346,7 @@
     </row>
     <row r="34" spans="1:15">
       <c r="A34" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="B34">
         <v>0.999</v>
@@ -10512,7 +10948,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>69</v>
@@ -10655,7 +11091,7 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="B13">
         <v>0.3</v>
@@ -10693,7 +11129,7 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="B14" s="3">
         <v>0.55000000000000004</v>
@@ -10731,7 +11167,7 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="B15" s="3">
         <v>0.99</v>
@@ -10739,7 +11175,7 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="B16" s="3">
         <v>0.999</v>
@@ -11211,7 +11647,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="B1">
         <v>0.15</v>
@@ -11240,92 +11676,92 @@
     </row>
     <row r="5" spans="1:2">
       <c r="B5" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="B6" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="B7" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="B8" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="B9" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="B10" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="B11" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="B12" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="B13" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="B14" t="s">
-        <v>196</v>
+        <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="B15" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="B16" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="B17" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="B18" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="B19" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="B20" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="B21" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="B22" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
     </row>
     <row r="23" spans="1:6">

</xml_diff>

<commit_message>
Update for additional FNetF SubBucket fields added for reg. reporting.  Clean up DRC CRIF->FNetF field mappings; allow both variants for DRC_CC.  Add more tests for SA-DRC.
</commit_message>
<xml_diff>
--- a/Configs/FRTBConfig_BCBS.xlsx
+++ b/Configs/FRTBConfig_BCBS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alan/Workspace/FRTB/Configs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08997159-1E7C-5247-85BB-940817035216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F6E0315-E0B7-7D4D-B3C3-220A4AAC82A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="76820" yWindow="10600" windowWidth="40140" windowHeight="26920" activeTab="11" xr2:uid="{702274BA-38C3-0147-8564-8B67C0FD49FC}"/>
+    <workbookView xWindow="111440" yWindow="15480" windowWidth="40140" windowHeight="26960" xr2:uid="{702274BA-38C3-0147-8564-8B67C0FD49FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Copyright" sheetId="22" r:id="rId1"/>
@@ -764,9 +764,6 @@
     <t>ReportingCurrency</t>
   </si>
   <si>
-    <t>Copyright (C) 2024 frtb.net limited</t>
-  </si>
-  <si>
     <t>Contact us at &lt;info@frtb.net&gt; or via our website at &lt;https://frtb.net&gt;</t>
   </si>
   <si>
@@ -867,6 +864,9 @@
   </si>
   <si>
     <t>Others</t>
+  </si>
+  <si>
+    <t>Copyright (C) 2024-2025 frtb.net limited</t>
   </si>
 </sst>
 </file>
@@ -1299,7 +1299,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D95B6A-2092-4D43-ABCB-456863E81D66}">
   <dimension ref="A1:A17"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1307,7 +1307,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="10" t="s">
-        <v>216</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -1315,7 +1315,7 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:1">
@@ -1326,22 +1326,22 @@
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:1">
@@ -1349,22 +1349,22 @@
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:1">
@@ -1372,12 +1372,12 @@
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -1637,12 +1637,14 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1653,7 +1655,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
@@ -1664,10 +1666,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D2" t="s">
         <v>236</v>
-      </c>
-      <c r="D2" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1678,7 +1680,7 @@
         <v>108</v>
       </c>
       <c r="D3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1689,7 +1691,7 @@
         <v>108</v>
       </c>
       <c r="D4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1700,7 +1702,7 @@
         <v>108</v>
       </c>
       <c r="D5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1711,7 +1713,7 @@
         <v>108</v>
       </c>
       <c r="D6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1722,7 +1724,7 @@
         <v>108</v>
       </c>
       <c r="D7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1733,7 +1735,7 @@
         <v>108</v>
       </c>
       <c r="D8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1744,7 +1746,7 @@
         <v>108</v>
       </c>
       <c r="D9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1755,7 +1757,7 @@
         <v>108</v>
       </c>
       <c r="D10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1766,7 +1768,7 @@
         <v>108</v>
       </c>
       <c r="D11" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1777,7 +1779,7 @@
         <v>108</v>
       </c>
       <c r="D12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1788,7 +1790,7 @@
         <v>108</v>
       </c>
       <c r="D13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1799,7 +1801,7 @@
         <v>109</v>
       </c>
       <c r="D14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1810,7 +1812,7 @@
         <v>109</v>
       </c>
       <c r="D15" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1821,7 +1823,7 @@
         <v>109</v>
       </c>
       <c r="D16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="2:4">
@@ -1832,7 +1834,7 @@
         <v>109</v>
       </c>
       <c r="D17" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18" spans="2:4">
@@ -1843,7 +1845,7 @@
         <v>109</v>
       </c>
       <c r="D18" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="19" spans="2:4">
@@ -1854,7 +1856,7 @@
         <v>109</v>
       </c>
       <c r="D19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="20" spans="2:4">
@@ -1865,7 +1867,7 @@
         <v>109</v>
       </c>
       <c r="D20" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="21" spans="2:4">
@@ -1876,7 +1878,7 @@
         <v>109</v>
       </c>
       <c r="D21" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="22" spans="2:4">
@@ -1887,7 +1889,7 @@
         <v>109</v>
       </c>
       <c r="D22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23" spans="2:4">
@@ -1898,7 +1900,7 @@
         <v>109</v>
       </c>
       <c r="D23" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="24" spans="2:4">
@@ -1909,7 +1911,7 @@
         <v>109</v>
       </c>
       <c r="D24" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25" spans="2:4">
@@ -1920,7 +1922,7 @@
         <v>110</v>
       </c>
       <c r="D25" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="26" spans="2:4">
@@ -1931,7 +1933,7 @@
         <v>110</v>
       </c>
       <c r="D26" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="27" spans="2:4">
@@ -1942,7 +1944,7 @@
         <v>110</v>
       </c>
       <c r="D27" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="28" spans="2:4">
@@ -1953,7 +1955,7 @@
         <v>110</v>
       </c>
       <c r="D28" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="29" spans="2:4">
@@ -1964,7 +1966,7 @@
         <v>110</v>
       </c>
       <c r="D29" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="30" spans="2:4">
@@ -1975,7 +1977,7 @@
         <v>110</v>
       </c>
       <c r="D30" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="31" spans="2:4">
@@ -1986,7 +1988,7 @@
         <v>110</v>
       </c>
       <c r="D31" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="32" spans="2:4">
@@ -1997,7 +1999,7 @@
         <v>110</v>
       </c>
       <c r="D32" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="33" spans="2:4">
@@ -2008,7 +2010,7 @@
         <v>110</v>
       </c>
       <c r="D33" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="34" spans="2:4">
@@ -2019,7 +2021,7 @@
         <v>110</v>
       </c>
       <c r="D34" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="35" spans="2:4">
@@ -2030,7 +2032,7 @@
         <v>110</v>
       </c>
       <c r="D35" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="36" spans="2:4">
@@ -2038,10 +2040,10 @@
         <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D36" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="37" spans="2:4">
@@ -2049,10 +2051,10 @@
         <v>36</v>
       </c>
       <c r="C37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D37" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="38" spans="2:4">
@@ -2060,10 +2062,10 @@
         <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D38" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="39" spans="2:4">
@@ -2071,10 +2073,10 @@
         <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D39" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="40" spans="2:4">
@@ -2082,10 +2084,10 @@
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D40" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="41" spans="2:4">
@@ -2093,10 +2095,10 @@
         <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D41" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="42" spans="2:4">
@@ -2104,10 +2106,10 @@
         <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D42" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="43" spans="2:4">
@@ -2115,10 +2117,10 @@
         <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D43" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="44" spans="2:4">
@@ -2126,10 +2128,10 @@
         <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D44" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="45" spans="2:4">
@@ -2137,10 +2139,10 @@
         <v>44</v>
       </c>
       <c r="C45" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D45" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="46" spans="2:4">
@@ -2148,10 +2150,10 @@
         <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D46" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="47" spans="2:4">
@@ -2159,10 +2161,10 @@
         <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D47" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -3314,9 +3316,7 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O19" sqref="O19:R19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -3512,7 +3512,7 @@
         <v>15</v>
       </c>
       <c r="E17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -3523,7 +3523,7 @@
         <v>118</v>
       </c>
       <c r="E18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="19" spans="1:18">
@@ -6863,7 +6863,7 @@
         <v>6</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -6877,7 +6877,7 @@
         <v>6</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -6997,10 +6997,10 @@
         <v>188</v>
       </c>
       <c r="I20" t="s">
+        <v>227</v>
+      </c>
+      <c r="J20" t="s">
         <v>228</v>
-      </c>
-      <c r="J20" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="21" spans="1:20">
@@ -10117,7 +10117,7 @@
         <v>47</v>
       </c>
       <c r="J14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -11721,7 +11721,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="B14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="15" spans="1:2">

</xml_diff>

<commit_message>
Tweaks to RRAO field names for consistency
</commit_message>
<xml_diff>
--- a/Configs/FRTBConfig_BCBS.xlsx
+++ b/Configs/FRTBConfig_BCBS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alan/Workspace/FRTB/Configs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F6E0315-E0B7-7D4D-B3C3-220A4AAC82A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACB3641-C007-9447-A247-A87A575FFEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="111440" yWindow="15480" windowWidth="40140" windowHeight="26960" xr2:uid="{702274BA-38C3-0147-8564-8B67C0FD49FC}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="285">
   <si>
     <t>Bucket</t>
   </si>
@@ -868,12 +868,114 @@
   <si>
     <t>Copyright (C) 2024-2025 frtb.net limited</t>
   </si>
+  <si>
+    <t>Buckets</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>FutureVol</t>
+  </si>
+  <si>
+    <t>Future realised volatility</t>
+  </si>
+  <si>
+    <t>NaturalDisaster</t>
+  </si>
+  <si>
+    <t>Natural disasters</t>
+  </si>
+  <si>
+    <t>Weather</t>
+  </si>
+  <si>
+    <t>Longevity</t>
+  </si>
+  <si>
+    <t>Longevity risk</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Other exotic underlyings which are not in the scope of the delta, vega or curvature risk</t>
+  </si>
+  <si>
+    <t>PathDependent</t>
+  </si>
+  <si>
+    <t>Options where the pay-offs depend on the path followed by the price of the underlying asset and not just its final price on the exercise date</t>
+  </si>
+  <si>
+    <t>FutureStrike</t>
+  </si>
+  <si>
+    <t>Options that start at a predefined date in the future and whose strike price is not yet determined at the time at which the option is in the trading book of the institution</t>
+  </si>
+  <si>
+    <t>OptionOnOption</t>
+  </si>
+  <si>
+    <t>Options whose underlying is another option</t>
+  </si>
+  <si>
+    <t>Discontinuious</t>
+  </si>
+  <si>
+    <t>Options with discontinuous pay-offs</t>
+  </si>
+  <si>
+    <t>VarialbleTerms</t>
+  </si>
+  <si>
+    <t>Options allowing the holder to modify the strike price or other terms of the contract before the maturity of the option</t>
+  </si>
+  <si>
+    <t>Bermudan</t>
+  </si>
+  <si>
+    <t>Options that can be exercised on a finite set of predetermined dates</t>
+  </si>
+  <si>
+    <t>XCcy</t>
+  </si>
+  <si>
+    <t>Options whose underlying is denominated in one currency but whose pay-offs are settled in a different currency, with a predetermined exchange rate between the two currencies</t>
+  </si>
+  <si>
+    <t>MultiUnderlier</t>
+  </si>
+  <si>
+    <t>Multi-underlying options</t>
+  </si>
+  <si>
+    <t>Behavioural</t>
+  </si>
+  <si>
+    <t>Options subject to behavioural risk</t>
+  </si>
+  <si>
+    <t>OpenMaturity</t>
+  </si>
+  <si>
+    <t>Options that do not have a maturity</t>
+  </si>
+  <si>
+    <t>MultiBarrier</t>
+  </si>
+  <si>
+    <t>Options that do not have a strike or barrier and options that have multiple strikes or barriers</t>
+  </si>
+  <si>
+    <t>Other instruments exposed to residual risk</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -935,6 +1037,12 @@
       <color rgb="FFFF0000"/>
       <name val="Source Code Pro"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -969,7 +1077,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -982,6 +1090,12 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2175,28 +2289,229 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C708CD6-DEC9-194A-B3B9-9CA14913B1F0}">
   <sheetPr codeName="Sheet12"/>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="B2" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="B3" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="B6" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="B8" t="s">
+        <v>198</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" t="s">
+        <v>198</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="B10" t="s">
+        <v>198</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="B11" t="s">
+        <v>198</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12" t="s">
+        <v>198</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="B13" t="s">
+        <v>198</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="B14" t="s">
+        <v>198</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="B15" t="s">
+        <v>198</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="B16" t="s">
+        <v>198</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="B17" t="s">
+        <v>198</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="B18" t="s">
+        <v>198</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
         <v>196</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B19" t="s">
         <v>197</v>
       </c>
-      <c r="C1">
+      <c r="C19">
         <v>0.01</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="B2" t="s">
+    <row r="20" spans="1:4">
+      <c r="B20" t="s">
         <v>198</v>
       </c>
-      <c r="C2">
+      <c r="C20">
         <v>1E-3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Rating column to Securitiations DRC; make config file parsing  tolerant of missing columns; In DRC factor out applyRiskWeights to parent class.
</commit_message>
<xml_diff>
--- a/Configs/FRTBConfig_BCBS.xlsx
+++ b/Configs/FRTBConfig_BCBS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alan/Workspace/FRTB/Configs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACB3641-C007-9447-A247-A87A575FFEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424FE1C9-BD15-E049-8A01-7FE14E24F5A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="111440" yWindow="15480" windowWidth="40140" windowHeight="26960" xr2:uid="{702274BA-38C3-0147-8564-8B67C0FD49FC}"/>
+    <workbookView xWindow="111540" yWindow="15420" windowWidth="40140" windowHeight="26960" xr2:uid="{702274BA-38C3-0147-8564-8B67C0FD49FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Copyright" sheetId="22" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="285">
   <si>
     <t>Bucket</t>
   </si>
@@ -1749,7 +1749,7 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5213FE0F-D032-134C-8CBD-C9C991BBB3F3}">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2116,7 +2116,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="33" spans="2:4">
+    <row r="33" spans="1:4">
       <c r="B33">
         <v>32</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="34" spans="2:4">
+    <row r="34" spans="1:4">
       <c r="B34">
         <v>33</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="35" spans="2:4">
+    <row r="35" spans="1:4">
       <c r="B35">
         <v>34</v>
       </c>
@@ -2149,7 +2149,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="36" spans="2:4">
+    <row r="36" spans="1:4">
       <c r="B36">
         <v>35</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="37" spans="2:4">
+    <row r="37" spans="1:4">
       <c r="B37">
         <v>36</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="38" spans="2:4">
+    <row r="38" spans="1:4">
       <c r="B38">
         <v>37</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="39" spans="2:4">
+    <row r="39" spans="1:4">
       <c r="B39">
         <v>38</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="40" spans="2:4">
+    <row r="40" spans="1:4">
       <c r="B40">
         <v>39</v>
       </c>
@@ -2204,7 +2204,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="41" spans="2:4">
+    <row r="41" spans="1:4">
       <c r="B41">
         <v>40</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="42" spans="2:4">
+    <row r="42" spans="1:4">
       <c r="B42">
         <v>41</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="43" spans="2:4">
+    <row r="43" spans="1:4">
       <c r="B43">
         <v>42</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="44" spans="2:4">
+    <row r="44" spans="1:4">
       <c r="B44">
         <v>43</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="45" spans="2:4">
+    <row r="45" spans="1:4">
       <c r="B45">
         <v>44</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="46" spans="2:4">
+    <row r="46" spans="1:4">
       <c r="B46">
         <v>45</v>
       </c>
@@ -2270,7 +2270,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="47" spans="2:4">
+    <row r="47" spans="1:4">
       <c r="B47">
         <v>46</v>
       </c>
@@ -2279,6 +2279,89 @@
       </c>
       <c r="D47" t="s">
         <v>249</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>100</v>
+      </c>
+      <c r="B48" t="s">
+        <v>101</v>
+      </c>
+      <c r="C48">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3">
+      <c r="B49" t="s">
+        <v>102</v>
+      </c>
+      <c r="C49">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3">
+      <c r="B50" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3">
+      <c r="B51" t="s">
+        <v>104</v>
+      </c>
+      <c r="C51">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3">
+      <c r="B52" t="s">
+        <v>105</v>
+      </c>
+      <c r="C52">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3">
+      <c r="B53" t="s">
+        <v>106</v>
+      </c>
+      <c r="C53">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3">
+      <c r="B54" t="s">
+        <v>107</v>
+      </c>
+      <c r="C54">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3">
+      <c r="B55" t="s">
+        <v>199</v>
+      </c>
+      <c r="C55">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3">
+      <c r="B56" t="s">
+        <v>200</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3">
+      <c r="B57" t="s">
+        <v>201</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -9708,9 +9791,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:Z34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>

</xml_diff>

<commit_message>
Add CQRiskWeights to BCBS MD_CS config
</commit_message>
<xml_diff>
--- a/Configs/FRTBConfig_BCBS.xlsx
+++ b/Configs/FRTBConfig_BCBS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alan/Workspace/FRTB/Configs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424FE1C9-BD15-E049-8A01-7FE14E24F5A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FD88D7-D64C-BF4C-98A7-1D6AC71ED536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="111540" yWindow="15420" windowWidth="40140" windowHeight="26960" xr2:uid="{702274BA-38C3-0147-8564-8B67C0FD49FC}"/>
+    <workbookView xWindow="2880" yWindow="1780" windowWidth="40140" windowHeight="26960" activeTab="12" xr2:uid="{702274BA-38C3-0147-8564-8B67C0FD49FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Copyright" sheetId="22" r:id="rId1"/>
@@ -1413,7 +1413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D95B6A-2092-4D43-ABCB-456863E81D66}">
   <dimension ref="A1:A17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2374,9 +2374,12 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -5885,7 +5888,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>

</xml_diff>

<commit_message>
Add CQRiskWeight to MD_CS; Bring Bucket config for MD_RR into conformity with other RiskClass configs.
</commit_message>
<xml_diff>
--- a/Configs/FRTBConfig_BCBS.xlsx
+++ b/Configs/FRTBConfig_BCBS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alan/Workspace/FRTB/Configs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FD88D7-D64C-BF4C-98A7-1D6AC71ED536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4144D5-3EFC-4C4C-B653-0CC29BAF3BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="1780" windowWidth="40140" windowHeight="26960" activeTab="12" xr2:uid="{702274BA-38C3-0147-8564-8B67C0FD49FC}"/>
+    <workbookView xWindow="2880" yWindow="1780" windowWidth="40140" windowHeight="26960" xr2:uid="{702274BA-38C3-0147-8564-8B67C0FD49FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Copyright" sheetId="22" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="284">
   <si>
     <t>Bucket</t>
   </si>
@@ -867,9 +867,6 @@
   </si>
   <si>
     <t>Copyright (C) 2024-2025 frtb.net limited</t>
-  </si>
-  <si>
-    <t>Buckets</t>
   </si>
   <si>
     <t>Description</t>
@@ -1413,7 +1410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D95B6A-2092-4D43-ABCB-456863E81D66}">
   <dimension ref="A1:A17"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2374,7 +2371,7 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -2383,7 +2380,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>251</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2392,7 +2389,7 @@
         <v>189</v>
       </c>
       <c r="D1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2400,10 +2397,10 @@
         <v>197</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>253</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2411,10 +2408,10 @@
         <v>197</v>
       </c>
       <c r="C3" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>255</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2422,10 +2419,10 @@
         <v>197</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2433,10 +2430,10 @@
         <v>197</v>
       </c>
       <c r="C5" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>258</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2444,10 +2441,10 @@
         <v>197</v>
       </c>
       <c r="C6" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>260</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2455,10 +2452,10 @@
         <v>198</v>
       </c>
       <c r="C7" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>262</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2466,10 +2463,10 @@
         <v>198</v>
       </c>
       <c r="C8" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>264</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2477,10 +2474,10 @@
         <v>198</v>
       </c>
       <c r="C9" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>266</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2488,10 +2485,10 @@
         <v>198</v>
       </c>
       <c r="C10" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>268</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2499,10 +2496,10 @@
         <v>198</v>
       </c>
       <c r="C11" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>270</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2510,10 +2507,10 @@
         <v>198</v>
       </c>
       <c r="C12" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="D12" s="13" t="s">
         <v>272</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2521,10 +2518,10 @@
         <v>198</v>
       </c>
       <c r="C13" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="D13" s="13" t="s">
         <v>274</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2532,10 +2529,10 @@
         <v>198</v>
       </c>
       <c r="C14" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="D14" s="13" t="s">
         <v>276</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2543,10 +2540,10 @@
         <v>198</v>
       </c>
       <c r="C15" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="D15" s="13" t="s">
         <v>278</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2554,10 +2551,10 @@
         <v>198</v>
       </c>
       <c r="C16" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="D16" s="13" t="s">
         <v>280</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2565,10 +2562,10 @@
         <v>198</v>
       </c>
       <c r="C17" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="D17" s="13" t="s">
         <v>282</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2576,10 +2573,10 @@
         <v>198</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -3179,9 +3176,7 @@
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -5888,9 +5883,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>

</xml_diff>